<commit_message>
Post-defense revisions: begin to look at things broken up by seasonality, so cool-season plants are matched with spring monitoring events, and warm-season plants are matched with fall monitoring events (year-round species retain all monitoring events)
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/14.1b_edited1_Sonoran-species-with-seasonality.xlsx
+++ b/data/data-wrangling-intermediate/14.1b_edited1_Sonoran-species-with-seasonality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="673" documentId="8_{C086D125-03D2-4B39-A8D3-7C75A2FD56D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45D293BC-0C2C-482C-8383-6D598BE6591A}"/>
+  <xr:revisionPtr revIDLastSave="697" documentId="8_{C086D125-03D2-4B39-A8D3-7C75A2FD56D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F59FEC4-1700-4B70-8337-247E162ECCAF}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{A86D511D-D736-42D0-AAA0-4036FA7DE759}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3816" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3817" uniqueCount="943">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -2138,9 +2138,6 @@
     <t>A few ARPUs and young BOCUs mostly near/in the south half except for a smaller ARPU in the northwest and a BAMU just north of subplot</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>ARPU about 5 individuals and an individual BAMU resprouting at base</t>
   </si>
   <si>
@@ -2858,14 +2855,47 @@
     <t>https://swbiodiversity.org/seinet/taxa/index.php?taxon=Prosopis+velutina&amp;formsubmit=Search+Terms</t>
   </si>
   <si>
-    <t>`</t>
+    <r>
+      <t>Co</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ol</t>
+    </r>
+  </si>
+  <si>
+    <t>the three most common Panicum sp in AZ are all warm</t>
+  </si>
+  <si>
+    <r>
+      <t>Wa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rm</t>
+    </r>
+  </si>
+  <si>
+    <t>https://swbiodiversity.org/seinet/taxa/index.php?taxon=Eriogonum+deflexum&amp;formsubmit=Search+Terms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2900,6 +2930,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2922,7 +2959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2930,6 +2967,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2960,8 +2998,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>458932</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19570</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2976,8 +3014,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10361122" y="238645"/>
-          <a:ext cx="3467446" cy="871970"/>
+          <a:off x="10366317" y="237779"/>
+          <a:ext cx="3484765" cy="1438621"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3038,6 +3076,27 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
             <a:t>book</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>Seasonality in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>blue</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> = confirmed by EcoRestore plant list that Elise shared with me</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3376,9 +3435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA92F59-5528-4E2B-884D-D01DEFA9FE33}">
   <dimension ref="A1:I450"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G387" sqref="G387"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C374" sqref="C374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3471,7 +3530,7 @@
         <v>543</v>
       </c>
       <c r="I3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3874,7 +3933,7 @@
         <v>524</v>
       </c>
       <c r="I17" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -4343,7 +4402,7 @@
         <v>527</v>
       </c>
       <c r="I34" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -4423,7 +4482,7 @@
       <c r="F37" t="s">
         <v>10</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H37" t="s">
@@ -4452,7 +4511,7 @@
       <c r="F38" t="s">
         <v>10</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H38" t="s">
@@ -4481,7 +4540,7 @@
       <c r="F39" t="s">
         <v>10</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H39" t="s">
@@ -4510,7 +4569,7 @@
       <c r="F40" t="s">
         <v>10</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H40" t="s">
@@ -4580,7 +4639,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B43" t="s">
         <v>75</v>
@@ -4609,7 +4668,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B44" t="s">
         <v>75</v>
@@ -4638,7 +4697,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B45" t="s">
         <v>75</v>
@@ -4667,7 +4726,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B46" t="s">
         <v>75</v>
@@ -4696,7 +4755,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B47" t="s">
         <v>75</v>
@@ -4725,7 +4784,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B48" t="s">
         <v>75</v>
@@ -4783,7 +4842,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B50" t="s">
         <v>75</v>
@@ -4812,7 +4871,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B51" t="s">
         <v>75</v>
@@ -4841,7 +4900,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
@@ -4986,13 +5045,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>709</v>
+      </c>
+      <c r="B57" t="s">
+        <v>709</v>
+      </c>
+      <c r="C57" t="s">
         <v>710</v>
-      </c>
-      <c r="B57" t="s">
-        <v>710</v>
-      </c>
-      <c r="C57" t="s">
-        <v>711</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -5010,7 +5069,7 @@
         <v>565</v>
       </c>
       <c r="I57" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -5186,13 +5245,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>711</v>
+      </c>
+      <c r="B64" t="s">
         <v>712</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>713</v>
-      </c>
-      <c r="C64" t="s">
-        <v>714</v>
       </c>
       <c r="D64" t="s">
         <v>3</v>
@@ -5207,10 +5266,10 @@
         <v>508</v>
       </c>
       <c r="H64" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I64" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -5290,8 +5349,8 @@
       <c r="F67" t="s">
         <v>10</v>
       </c>
-      <c r="G67" t="s">
-        <v>524</v>
+      <c r="G67" s="5" t="s">
+        <v>681</v>
       </c>
       <c r="H67" t="s">
         <v>572</v>
@@ -5439,7 +5498,7 @@
         <v>15</v>
       </c>
       <c r="I72" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -5447,11 +5506,11 @@
         <v>112</v>
       </c>
       <c r="B73" t="s">
+        <v>714</v>
+      </c>
+      <c r="C73" t="s">
         <v>715</v>
       </c>
-      <c r="C73" t="s">
-        <v>716</v>
-      </c>
       <c r="D73" t="s">
         <v>3</v>
       </c>
@@ -5465,7 +5524,7 @@
         <v>15</v>
       </c>
       <c r="I73" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -5491,7 +5550,7 @@
         <v>15</v>
       </c>
       <c r="I74" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -5517,7 +5576,7 @@
         <v>15</v>
       </c>
       <c r="I75" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -5543,7 +5602,7 @@
         <v>15</v>
       </c>
       <c r="I76" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -5569,7 +5628,7 @@
         <v>15</v>
       </c>
       <c r="I77" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -5595,7 +5654,7 @@
         <v>15</v>
       </c>
       <c r="I78" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -5687,10 +5746,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B82" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C82" t="s">
         <v>695</v>
@@ -5708,10 +5767,10 @@
         <v>681</v>
       </c>
       <c r="H82" t="s">
+        <v>914</v>
+      </c>
+      <c r="I82" t="s">
         <v>915</v>
-      </c>
-      <c r="I82" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -5774,13 +5833,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>717</v>
+      </c>
+      <c r="B85" t="s">
+        <v>717</v>
+      </c>
+      <c r="C85" t="s">
         <v>718</v>
-      </c>
-      <c r="B85" t="s">
-        <v>718</v>
-      </c>
-      <c r="C85" t="s">
-        <v>719</v>
       </c>
       <c r="D85" t="s">
         <v>3</v>
@@ -5792,13 +5851,13 @@
         <v>10</v>
       </c>
       <c r="G85" t="s">
-        <v>700</v>
+        <v>681</v>
       </c>
       <c r="H85" t="s">
-        <v>700</v>
+        <v>527</v>
       </c>
       <c r="I85" t="s">
-        <v>700</v>
+        <v>942</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -6040,13 +6099,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>719</v>
+      </c>
+      <c r="B95" t="s">
+        <v>719</v>
+      </c>
+      <c r="C95" t="s">
         <v>720</v>
-      </c>
-      <c r="B95" t="s">
-        <v>720</v>
-      </c>
-      <c r="C95" t="s">
-        <v>721</v>
       </c>
       <c r="D95" t="s">
         <v>3</v>
@@ -6219,13 +6278,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>721</v>
+      </c>
+      <c r="B102" t="s">
+        <v>721</v>
+      </c>
+      <c r="C102" t="s">
         <v>722</v>
-      </c>
-      <c r="B102" t="s">
-        <v>722</v>
-      </c>
-      <c r="C102" t="s">
-        <v>723</v>
       </c>
       <c r="D102" t="s">
         <v>3</v>
@@ -6240,10 +6299,10 @@
         <v>524</v>
       </c>
       <c r="H102" t="s">
+        <v>916</v>
+      </c>
+      <c r="I102" t="s">
         <v>917</v>
-      </c>
-      <c r="I102" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -6277,13 +6336,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>723</v>
+      </c>
+      <c r="B104" t="s">
         <v>724</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>725</v>
-      </c>
-      <c r="C104" t="s">
-        <v>726</v>
       </c>
       <c r="D104" t="s">
         <v>3</v>
@@ -6301,7 +6360,7 @@
         <v>514</v>
       </c>
       <c r="I104" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -6816,7 +6875,7 @@
       <c r="F122" t="s">
         <v>10</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H122" t="s">
@@ -6828,7 +6887,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B123" t="s">
         <v>211</v>
@@ -6845,7 +6904,7 @@
       <c r="F123" t="s">
         <v>10</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H123" t="s">
@@ -6857,7 +6916,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B124" t="s">
         <v>211</v>
@@ -6874,7 +6933,7 @@
       <c r="F124" t="s">
         <v>10</v>
       </c>
-      <c r="G124" t="s">
+      <c r="G124" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H124" t="s">
@@ -6886,7 +6945,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B125" t="s">
         <v>211</v>
@@ -6903,7 +6962,7 @@
       <c r="F125" t="s">
         <v>10</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H125" t="s">
@@ -6915,7 +6974,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B126" t="s">
         <v>211</v>
@@ -6932,7 +6991,7 @@
       <c r="F126" t="s">
         <v>10</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H126" t="s">
@@ -6944,7 +7003,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B127" t="s">
         <v>211</v>
@@ -6961,7 +7020,7 @@
       <c r="F127" t="s">
         <v>10</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H127" t="s">
@@ -6973,7 +7032,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B128" t="s">
         <v>211</v>
@@ -6990,7 +7049,7 @@
       <c r="F128" t="s">
         <v>10</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G128" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H128" t="s">
@@ -7002,7 +7061,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B129" t="s">
         <v>211</v>
@@ -7019,7 +7078,7 @@
       <c r="F129" t="s">
         <v>10</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G129" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H129" t="s">
@@ -7031,7 +7090,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B130" t="s">
         <v>211</v>
@@ -7048,7 +7107,7 @@
       <c r="F130" t="s">
         <v>10</v>
       </c>
-      <c r="G130" t="s">
+      <c r="G130" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H130" t="s">
@@ -7060,7 +7119,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B131" t="s">
         <v>211</v>
@@ -7077,7 +7136,7 @@
       <c r="F131" t="s">
         <v>10</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G131" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H131" t="s">
@@ -7164,13 +7223,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>735</v>
+      </c>
+      <c r="B135" t="s">
         <v>736</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>737</v>
-      </c>
-      <c r="C135" t="s">
-        <v>738</v>
       </c>
       <c r="D135" t="s">
         <v>3</v>
@@ -7185,10 +7244,10 @@
         <v>508</v>
       </c>
       <c r="H135" t="s">
+        <v>919</v>
+      </c>
+      <c r="I135" t="s">
         <v>920</v>
-      </c>
-      <c r="I135" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -7214,7 +7273,7 @@
         <v>508</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="I136" t="s">
         <v>683</v>
@@ -7303,14 +7362,14 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>738</v>
+      </c>
+      <c r="B140" t="s">
         <v>739</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>740</v>
       </c>
-      <c r="C140" t="s">
-        <v>741</v>
-      </c>
       <c r="D140" t="s">
         <v>3</v>
       </c>
@@ -7324,22 +7383,22 @@
         <v>524</v>
       </c>
       <c r="H140" t="s">
+        <v>921</v>
+      </c>
+      <c r="I140" t="s">
         <v>922</v>
-      </c>
-      <c r="I140" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B141" t="s">
+        <v>739</v>
+      </c>
+      <c r="C141" t="s">
         <v>740</v>
       </c>
-      <c r="C141" t="s">
-        <v>741</v>
-      </c>
       <c r="D141" t="s">
         <v>3</v>
       </c>
@@ -7353,22 +7412,22 @@
         <v>524</v>
       </c>
       <c r="H141" t="s">
+        <v>921</v>
+      </c>
+      <c r="I141" t="s">
         <v>922</v>
-      </c>
-      <c r="I141" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B142" t="s">
+        <v>739</v>
+      </c>
+      <c r="C142" t="s">
         <v>740</v>
       </c>
-      <c r="C142" t="s">
-        <v>741</v>
-      </c>
       <c r="D142" t="s">
         <v>3</v>
       </c>
@@ -7382,10 +7441,10 @@
         <v>524</v>
       </c>
       <c r="H142" t="s">
+        <v>921</v>
+      </c>
+      <c r="I142" t="s">
         <v>922</v>
-      </c>
-      <c r="I142" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
@@ -7477,13 +7536,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>743</v>
+      </c>
+      <c r="B146" t="s">
         <v>744</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>745</v>
-      </c>
-      <c r="C146" t="s">
-        <v>746</v>
       </c>
       <c r="D146" t="s">
         <v>3</v>
@@ -7737,7 +7796,7 @@
       <c r="F155" t="s">
         <v>10</v>
       </c>
-      <c r="G155" t="s">
+      <c r="G155" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H155" t="s">
@@ -7749,7 +7808,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B156" t="s">
         <v>251</v>
@@ -7766,7 +7825,7 @@
       <c r="F156" t="s">
         <v>10</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G156" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H156" t="s">
@@ -7778,7 +7837,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B157" t="s">
         <v>251</v>
@@ -7795,7 +7854,7 @@
       <c r="F157" t="s">
         <v>10</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G157" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H157" t="s">
@@ -7807,7 +7866,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B158" t="s">
         <v>251</v>
@@ -7824,7 +7883,7 @@
       <c r="F158" t="s">
         <v>10</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G158" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H158" t="s">
@@ -7836,7 +7895,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B159" t="s">
         <v>251</v>
@@ -7853,7 +7912,7 @@
       <c r="F159" t="s">
         <v>10</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G159" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H159" t="s">
@@ -7865,7 +7924,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B160" t="s">
         <v>251</v>
@@ -7882,7 +7941,7 @@
       <c r="F160" t="s">
         <v>10</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G160" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H160" t="s">
@@ -7911,7 +7970,7 @@
       <c r="F161" t="s">
         <v>10</v>
       </c>
-      <c r="G161" t="s">
+      <c r="G161" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H161" t="s">
@@ -7923,7 +7982,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B162" t="s">
         <v>251</v>
@@ -7940,7 +7999,7 @@
       <c r="F162" t="s">
         <v>10</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G162" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H162" t="s">
@@ -7952,7 +8011,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B163" t="s">
         <v>251</v>
@@ -7969,7 +8028,7 @@
       <c r="F163" t="s">
         <v>10</v>
       </c>
-      <c r="G163" t="s">
+      <c r="G163" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H163" t="s">
@@ -7981,7 +8040,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B164" t="s">
         <v>251</v>
@@ -7998,7 +8057,7 @@
       <c r="F164" t="s">
         <v>10</v>
       </c>
-      <c r="G164" t="s">
+      <c r="G164" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H164" t="s">
@@ -8010,7 +8069,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B165" t="s">
         <v>251</v>
@@ -8027,7 +8086,7 @@
       <c r="F165" t="s">
         <v>10</v>
       </c>
-      <c r="G165" t="s">
+      <c r="G165" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H165" t="s">
@@ -8039,7 +8098,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B166" t="s">
         <v>251</v>
@@ -8056,7 +8115,7 @@
       <c r="F166" t="s">
         <v>10</v>
       </c>
-      <c r="G166" t="s">
+      <c r="G166" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H166" t="s">
@@ -8068,7 +8127,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B167" t="s">
         <v>251</v>
@@ -8085,7 +8144,7 @@
       <c r="F167" t="s">
         <v>10</v>
       </c>
-      <c r="G167" t="s">
+      <c r="G167" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H167" t="s">
@@ -8114,7 +8173,7 @@
       <c r="F168" t="s">
         <v>10</v>
       </c>
-      <c r="G168" t="s">
+      <c r="G168" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H168" t="s">
@@ -8126,7 +8185,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B169" t="s">
         <v>251</v>
@@ -8143,7 +8202,7 @@
       <c r="F169" t="s">
         <v>10</v>
       </c>
-      <c r="G169" t="s">
+      <c r="G169" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H169" t="s">
@@ -8172,7 +8231,7 @@
       <c r="F170" t="s">
         <v>10</v>
       </c>
-      <c r="G170" t="s">
+      <c r="G170" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H170" t="s">
@@ -8184,7 +8243,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B171" t="s">
         <v>251</v>
@@ -8201,7 +8260,7 @@
       <c r="F171" t="s">
         <v>10</v>
       </c>
-      <c r="G171" t="s">
+      <c r="G171" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H171" t="s">
@@ -8213,7 +8272,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B172" t="s">
         <v>251</v>
@@ -8230,7 +8289,7 @@
       <c r="F172" t="s">
         <v>10</v>
       </c>
-      <c r="G172" t="s">
+      <c r="G172" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H172" t="s">
@@ -8242,7 +8301,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B173" t="s">
         <v>251</v>
@@ -8259,7 +8318,7 @@
       <c r="F173" t="s">
         <v>10</v>
       </c>
-      <c r="G173" t="s">
+      <c r="G173" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H173" t="s">
@@ -8271,7 +8330,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B174" t="s">
         <v>251</v>
@@ -8288,7 +8347,7 @@
       <c r="F174" t="s">
         <v>10</v>
       </c>
-      <c r="G174" t="s">
+      <c r="G174" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H174" t="s">
@@ -8300,7 +8359,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B175" t="s">
         <v>251</v>
@@ -8317,7 +8376,7 @@
       <c r="F175" t="s">
         <v>10</v>
       </c>
-      <c r="G175" t="s">
+      <c r="G175" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H175" t="s">
@@ -8329,7 +8388,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B176" t="s">
         <v>251</v>
@@ -8346,7 +8405,7 @@
       <c r="F176" t="s">
         <v>10</v>
       </c>
-      <c r="G176" t="s">
+      <c r="G176" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H176" t="s">
@@ -8379,7 +8438,7 @@
         <v>508</v>
       </c>
       <c r="H177" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I177" t="s">
         <v>684</v>
@@ -8462,8 +8521,8 @@
       <c r="F180" t="s">
         <v>10</v>
       </c>
-      <c r="G180" s="2" t="s">
-        <v>524</v>
+      <c r="G180" s="5" t="s">
+        <v>508</v>
       </c>
       <c r="H180" t="s">
         <v>527</v>
@@ -8590,13 +8649,13 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>760</v>
+      </c>
+      <c r="B185" t="s">
+        <v>760</v>
+      </c>
+      <c r="C185" t="s">
         <v>761</v>
-      </c>
-      <c r="B185" t="s">
-        <v>761</v>
-      </c>
-      <c r="C185" t="s">
-        <v>762</v>
       </c>
       <c r="D185" t="s">
         <v>3</v>
@@ -8648,14 +8707,14 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>762</v>
+      </c>
+      <c r="B187" t="s">
         <v>763</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
         <v>764</v>
       </c>
-      <c r="C187" t="s">
-        <v>765</v>
-      </c>
       <c r="D187" t="s">
         <v>3</v>
       </c>
@@ -8669,22 +8728,22 @@
         <v>524</v>
       </c>
       <c r="H187" t="s">
+        <v>923</v>
+      </c>
+      <c r="I187" t="s">
         <v>924</v>
-      </c>
-      <c r="I187" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B188" t="s">
+        <v>763</v>
+      </c>
+      <c r="C188" t="s">
         <v>764</v>
       </c>
-      <c r="C188" t="s">
-        <v>765</v>
-      </c>
       <c r="D188" t="s">
         <v>3</v>
       </c>
@@ -8698,22 +8757,22 @@
         <v>524</v>
       </c>
       <c r="H188" t="s">
+        <v>923</v>
+      </c>
+      <c r="I188" t="s">
         <v>924</v>
-      </c>
-      <c r="I188" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B189" t="s">
+        <v>763</v>
+      </c>
+      <c r="C189" t="s">
         <v>764</v>
       </c>
-      <c r="C189" t="s">
-        <v>765</v>
-      </c>
       <c r="D189" t="s">
         <v>3</v>
       </c>
@@ -8727,22 +8786,22 @@
         <v>524</v>
       </c>
       <c r="H189" t="s">
+        <v>923</v>
+      </c>
+      <c r="I189" t="s">
         <v>924</v>
-      </c>
-      <c r="I189" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B190" t="s">
+        <v>763</v>
+      </c>
+      <c r="C190" t="s">
         <v>764</v>
       </c>
-      <c r="C190" t="s">
-        <v>765</v>
-      </c>
       <c r="D190" t="s">
         <v>3</v>
       </c>
@@ -8756,22 +8815,22 @@
         <v>524</v>
       </c>
       <c r="H190" t="s">
+        <v>923</v>
+      </c>
+      <c r="I190" t="s">
         <v>924</v>
-      </c>
-      <c r="I190" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B191" t="s">
+        <v>763</v>
+      </c>
+      <c r="C191" t="s">
         <v>764</v>
       </c>
-      <c r="C191" t="s">
-        <v>765</v>
-      </c>
       <c r="D191" t="s">
         <v>3</v>
       </c>
@@ -8785,22 +8844,22 @@
         <v>524</v>
       </c>
       <c r="H191" t="s">
+        <v>923</v>
+      </c>
+      <c r="I191" t="s">
         <v>924</v>
-      </c>
-      <c r="I191" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B192" t="s">
+        <v>763</v>
+      </c>
+      <c r="C192" t="s">
         <v>764</v>
       </c>
-      <c r="C192" t="s">
-        <v>765</v>
-      </c>
       <c r="D192" t="s">
         <v>3</v>
       </c>
@@ -8814,10 +8873,10 @@
         <v>524</v>
       </c>
       <c r="H192" t="s">
+        <v>923</v>
+      </c>
+      <c r="I192" t="s">
         <v>924</v>
-      </c>
-      <c r="I192" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
@@ -8839,7 +8898,7 @@
       <c r="F193" t="s">
         <v>34</v>
       </c>
-      <c r="G193" t="s">
+      <c r="G193" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H193" t="s">
@@ -8961,7 +9020,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B198" t="s">
         <v>279</v>
@@ -8990,7 +9049,7 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B199" t="s">
         <v>279</v>
@@ -9048,7 +9107,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B201" t="s">
         <v>279</v>
@@ -9077,7 +9136,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B202" t="s">
         <v>279</v>
@@ -9106,7 +9165,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B203" t="s">
         <v>279</v>
@@ -9135,7 +9194,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B204" t="s">
         <v>279</v>
@@ -9164,7 +9223,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B205" t="s">
         <v>279</v>
@@ -9193,7 +9252,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B206" t="s">
         <v>279</v>
@@ -9222,7 +9281,7 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B207" t="s">
         <v>279</v>
@@ -9251,7 +9310,7 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B208" t="s">
         <v>279</v>
@@ -9280,7 +9339,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B209" t="s">
         <v>279</v>
@@ -9309,7 +9368,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B210" t="s">
         <v>279</v>
@@ -9338,7 +9397,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B211" t="s">
         <v>279</v>
@@ -9367,7 +9426,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B212" t="s">
         <v>279</v>
@@ -9396,7 +9455,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B213" t="s">
         <v>279</v>
@@ -9425,7 +9484,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B214" t="s">
         <v>279</v>
@@ -9454,7 +9513,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B215" t="s">
         <v>279</v>
@@ -9483,7 +9542,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B216" t="s">
         <v>279</v>
@@ -9512,7 +9571,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B217" t="s">
         <v>279</v>
@@ -9570,7 +9629,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B219" t="s">
         <v>279</v>
@@ -9599,7 +9658,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B220" t="s">
         <v>279</v>
@@ -9628,7 +9687,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B221" t="s">
         <v>279</v>
@@ -9657,7 +9716,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B222" t="s">
         <v>279</v>
@@ -9686,7 +9745,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B223" t="s">
         <v>279</v>
@@ -9715,7 +9774,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B224" t="s">
         <v>279</v>
@@ -9744,7 +9803,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B225" t="s">
         <v>279</v>
@@ -9773,7 +9832,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B226" t="s">
         <v>279</v>
@@ -9802,7 +9861,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B227" t="s">
         <v>279</v>
@@ -9860,7 +9919,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B229" t="s">
         <v>279</v>
@@ -9889,7 +9948,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B230" t="s">
         <v>279</v>
@@ -9918,7 +9977,7 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B231" t="s">
         <v>279</v>
@@ -9947,7 +10006,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B232" t="s">
         <v>279</v>
@@ -9976,7 +10035,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B233" t="s">
         <v>279</v>
@@ -10005,7 +10064,7 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B234" t="s">
         <v>279</v>
@@ -10034,7 +10093,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B235" t="s">
         <v>279</v>
@@ -10063,7 +10122,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B236" t="s">
         <v>279</v>
@@ -10092,7 +10151,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B237" t="s">
         <v>279</v>
@@ -10121,7 +10180,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B238" t="s">
         <v>279</v>
@@ -10150,7 +10209,7 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B239" t="s">
         <v>279</v>
@@ -10179,7 +10238,7 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B240" t="s">
         <v>279</v>
@@ -10208,7 +10267,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B241" t="s">
         <v>279</v>
@@ -10266,7 +10325,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B243" t="s">
         <v>279</v>
@@ -10295,7 +10354,7 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B244" t="s">
         <v>279</v>
@@ -10324,7 +10383,7 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B245" t="s">
         <v>279</v>
@@ -10353,7 +10412,7 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B246" t="s">
         <v>279</v>
@@ -10382,7 +10441,7 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B247" t="s">
         <v>279</v>
@@ -10411,7 +10470,7 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B248" t="s">
         <v>279</v>
@@ -10440,7 +10499,7 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B249" t="s">
         <v>279</v>
@@ -10469,7 +10528,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B250" t="s">
         <v>279</v>
@@ -10498,7 +10557,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B251" t="s">
         <v>279</v>
@@ -10527,7 +10586,7 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B252" t="s">
         <v>279</v>
@@ -10556,7 +10615,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B253" t="s">
         <v>279</v>
@@ -10585,7 +10644,7 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B254" t="s">
         <v>279</v>
@@ -10614,7 +10673,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B255" t="s">
         <v>279</v>
@@ -10643,7 +10702,7 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B256" t="s">
         <v>279</v>
@@ -10672,10 +10731,10 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B257" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C257" t="s">
         <v>278</v>
@@ -10698,10 +10757,10 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B258" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C258" t="s">
         <v>278</v>
@@ -10724,10 +10783,10 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B259" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C259" t="s">
         <v>278</v>
@@ -10805,13 +10864,13 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
+        <v>805</v>
+      </c>
+      <c r="B262" t="s">
+        <v>805</v>
+      </c>
+      <c r="C262" t="s">
         <v>806</v>
-      </c>
-      <c r="B262" t="s">
-        <v>806</v>
-      </c>
-      <c r="C262" t="s">
-        <v>807</v>
       </c>
       <c r="D262" t="s">
         <v>3</v>
@@ -10829,7 +10888,7 @@
         <v>616</v>
       </c>
       <c r="I262" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.3">
@@ -10863,7 +10922,7 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B264" t="s">
         <v>286</v>
@@ -10921,7 +10980,7 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B266" t="s">
         <v>286</v>
@@ -10950,7 +11009,7 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B267" t="s">
         <v>286</v>
@@ -10979,7 +11038,7 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B268" t="s">
         <v>286</v>
@@ -11008,7 +11067,7 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B269" t="s">
         <v>286</v>
@@ -11037,7 +11096,7 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B270" t="s">
         <v>286</v>
@@ -11066,7 +11125,7 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B271" t="s">
         <v>286</v>
@@ -11095,7 +11154,7 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B272" t="s">
         <v>286</v>
@@ -11124,7 +11183,7 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B273" t="s">
         <v>286</v>
@@ -11153,7 +11212,7 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B274" t="s">
         <v>286</v>
@@ -11182,7 +11241,7 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B275" t="s">
         <v>286</v>
@@ -11211,7 +11270,7 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B276" t="s">
         <v>286</v>
@@ -11240,7 +11299,7 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B277" t="s">
         <v>286</v>
@@ -11269,7 +11328,7 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B278" t="s">
         <v>286</v>
@@ -11298,7 +11357,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B279" t="s">
         <v>286</v>
@@ -11327,7 +11386,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B280" t="s">
         <v>286</v>
@@ -11356,7 +11415,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B281" t="s">
         <v>286</v>
@@ -11385,7 +11444,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B282" t="s">
         <v>286</v>
@@ -11414,7 +11473,7 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B283" t="s">
         <v>286</v>
@@ -11443,7 +11502,7 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B284" t="s">
         <v>286</v>
@@ -11472,7 +11531,7 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B285" t="s">
         <v>286</v>
@@ -11501,7 +11560,7 @@
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B286" t="s">
         <v>286</v>
@@ -11530,7 +11589,7 @@
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B287" t="s">
         <v>286</v>
@@ -11559,7 +11618,7 @@
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B288" t="s">
         <v>286</v>
@@ -11588,7 +11647,7 @@
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B289" t="s">
         <v>286</v>
@@ -11617,7 +11676,7 @@
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B290" t="s">
         <v>286</v>
@@ -11646,7 +11705,7 @@
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B291" t="s">
         <v>286</v>
@@ -11675,7 +11734,7 @@
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B292" t="s">
         <v>286</v>
@@ -11704,7 +11763,7 @@
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B293" t="s">
         <v>286</v>
@@ -11733,7 +11792,7 @@
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B294" t="s">
         <v>286</v>
@@ -11762,7 +11821,7 @@
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B295" t="s">
         <v>286</v>
@@ -11791,7 +11850,7 @@
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B296" t="s">
         <v>286</v>
@@ -11820,7 +11879,7 @@
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B297" t="s">
         <v>286</v>
@@ -11849,7 +11908,7 @@
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B298" t="s">
         <v>286</v>
@@ -11907,7 +11966,7 @@
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B300" t="s">
         <v>286</v>
@@ -11936,7 +11995,7 @@
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B301" t="s">
         <v>286</v>
@@ -11965,7 +12024,7 @@
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B302" t="s">
         <v>286</v>
@@ -11994,7 +12053,7 @@
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B303" t="s">
         <v>286</v>
@@ -12023,7 +12082,7 @@
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B304" t="s">
         <v>286</v>
@@ -12052,7 +12111,7 @@
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B305" t="s">
         <v>286</v>
@@ -12081,7 +12140,7 @@
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B306" t="s">
         <v>286</v>
@@ -12110,7 +12169,7 @@
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B307" t="s">
         <v>286</v>
@@ -12139,7 +12198,7 @@
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B308" t="s">
         <v>286</v>
@@ -12168,13 +12227,13 @@
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
+        <v>821</v>
+      </c>
+      <c r="B309" t="s">
         <v>822</v>
       </c>
-      <c r="B309" t="s">
+      <c r="C309" t="s">
         <v>823</v>
-      </c>
-      <c r="C309" t="s">
-        <v>824</v>
       </c>
       <c r="D309" t="s">
         <v>3</v>
@@ -12191,13 +12250,13 @@
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>824</v>
+      </c>
+      <c r="B310" t="s">
         <v>825</v>
       </c>
-      <c r="B310" t="s">
+      <c r="C310" t="s">
         <v>826</v>
-      </c>
-      <c r="C310" t="s">
-        <v>827</v>
       </c>
       <c r="D310" t="s">
         <v>3</v>
@@ -12214,13 +12273,13 @@
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B311" t="s">
+        <v>825</v>
+      </c>
+      <c r="C311" t="s">
         <v>826</v>
-      </c>
-      <c r="C311" t="s">
-        <v>827</v>
       </c>
       <c r="D311" t="s">
         <v>3</v>
@@ -12237,7 +12296,7 @@
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B312" t="s">
         <v>288</v>
@@ -12266,7 +12325,7 @@
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B313" t="s">
         <v>288</v>
@@ -12324,7 +12383,7 @@
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B315" t="s">
         <v>288</v>
@@ -12382,13 +12441,13 @@
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>831</v>
+      </c>
+      <c r="B317" t="s">
         <v>832</v>
       </c>
-      <c r="B317" t="s">
+      <c r="C317" t="s">
         <v>833</v>
-      </c>
-      <c r="C317" t="s">
-        <v>834</v>
       </c>
       <c r="D317" t="s">
         <v>3</v>
@@ -12406,18 +12465,18 @@
         <v>618</v>
       </c>
       <c r="I317" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B318" t="s">
+        <v>832</v>
+      </c>
+      <c r="C318" t="s">
         <v>833</v>
-      </c>
-      <c r="C318" t="s">
-        <v>834</v>
       </c>
       <c r="D318" t="s">
         <v>3</v>
@@ -12435,18 +12494,18 @@
         <v>618</v>
       </c>
       <c r="I318" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B319" t="s">
+        <v>832</v>
+      </c>
+      <c r="C319" t="s">
         <v>833</v>
-      </c>
-      <c r="C319" t="s">
-        <v>834</v>
       </c>
       <c r="D319" t="s">
         <v>3</v>
@@ -12464,18 +12523,18 @@
         <v>618</v>
       </c>
       <c r="I319" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B320" t="s">
+        <v>832</v>
+      </c>
+      <c r="C320" t="s">
         <v>833</v>
-      </c>
-      <c r="C320" t="s">
-        <v>834</v>
       </c>
       <c r="D320" t="s">
         <v>3</v>
@@ -12493,18 +12552,18 @@
         <v>618</v>
       </c>
       <c r="I320" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B321" t="s">
+        <v>832</v>
+      </c>
+      <c r="C321" t="s">
         <v>833</v>
-      </c>
-      <c r="C321" t="s">
-        <v>834</v>
       </c>
       <c r="D321" t="s">
         <v>3</v>
@@ -12522,18 +12581,18 @@
         <v>618</v>
       </c>
       <c r="I321" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B322" t="s">
+        <v>832</v>
+      </c>
+      <c r="C322" t="s">
         <v>833</v>
-      </c>
-      <c r="C322" t="s">
-        <v>834</v>
       </c>
       <c r="D322" t="s">
         <v>3</v>
@@ -12551,7 +12610,7 @@
         <v>618</v>
       </c>
       <c r="I322" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -12573,7 +12632,7 @@
       <c r="F323" t="s">
         <v>34</v>
       </c>
-      <c r="G323" t="s">
+      <c r="G323" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H323" t="s">
@@ -12585,10 +12644,10 @@
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>838</v>
+      </c>
+      <c r="B324" t="s">
         <v>839</v>
-      </c>
-      <c r="B324" t="s">
-        <v>840</v>
       </c>
       <c r="C324" t="s">
         <v>297</v>
@@ -12611,10 +12670,10 @@
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B325" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C325" t="s">
         <v>297</v>
@@ -12654,7 +12713,7 @@
       <c r="F326" t="s">
         <v>34</v>
       </c>
-      <c r="G326" t="s">
+      <c r="G326" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H326" t="s">
@@ -12692,13 +12751,13 @@
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>841</v>
+      </c>
+      <c r="B328" t="s">
         <v>842</v>
       </c>
-      <c r="B328" t="s">
+      <c r="C328" t="s">
         <v>843</v>
-      </c>
-      <c r="C328" t="s">
-        <v>844</v>
       </c>
       <c r="D328" t="s">
         <v>3</v>
@@ -12718,10 +12777,10 @@
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B329" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C329" t="s">
         <v>297</v>
@@ -12744,10 +12803,10 @@
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B330" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C330" t="s">
         <v>297</v>
@@ -12770,10 +12829,10 @@
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B331" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C331" t="s">
         <v>297</v>
@@ -12796,10 +12855,10 @@
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B332" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C332" t="s">
         <v>297</v>
@@ -12978,7 +13037,7 @@
       <c r="F338" t="s">
         <v>34</v>
       </c>
-      <c r="G338" t="s">
+      <c r="G338" s="5" t="s">
         <v>524</v>
       </c>
       <c r="H338" t="s">
@@ -13008,18 +13067,21 @@
         <v>34</v>
       </c>
       <c r="G339" t="s">
-        <v>15</v>
+        <v>524</v>
+      </c>
+      <c r="I339" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B340" t="s">
+        <v>848</v>
+      </c>
+      <c r="C340" t="s">
         <v>849</v>
-      </c>
-      <c r="C340" t="s">
-        <v>850</v>
       </c>
       <c r="D340" t="s">
         <v>3</v>
@@ -13037,18 +13099,18 @@
         <v>514</v>
       </c>
       <c r="I340" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B341" t="s">
+        <v>850</v>
+      </c>
+      <c r="C341" t="s">
         <v>851</v>
-      </c>
-      <c r="C341" t="s">
-        <v>852</v>
       </c>
       <c r="D341" t="s">
         <v>3</v>
@@ -13066,18 +13128,18 @@
         <v>527</v>
       </c>
       <c r="I341" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B342" t="s">
+        <v>850</v>
+      </c>
+      <c r="C342" t="s">
         <v>851</v>
-      </c>
-      <c r="C342" t="s">
-        <v>852</v>
       </c>
       <c r="D342" t="s">
         <v>3</v>
@@ -13095,18 +13157,18 @@
         <v>527</v>
       </c>
       <c r="I342" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B343" t="s">
+        <v>850</v>
+      </c>
+      <c r="C343" t="s">
         <v>851</v>
-      </c>
-      <c r="C343" t="s">
-        <v>852</v>
       </c>
       <c r="D343" t="s">
         <v>3</v>
@@ -13124,18 +13186,18 @@
         <v>527</v>
       </c>
       <c r="I343" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B344" t="s">
+        <v>850</v>
+      </c>
+      <c r="C344" t="s">
         <v>851</v>
-      </c>
-      <c r="C344" t="s">
-        <v>852</v>
       </c>
       <c r="D344" t="s">
         <v>3</v>
@@ -13153,7 +13215,7 @@
         <v>527</v>
       </c>
       <c r="I344" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -13208,12 +13270,12 @@
         <v>508</v>
       </c>
       <c r="I346" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B347" t="s">
         <v>316</v>
@@ -13234,12 +13296,12 @@
         <v>508</v>
       </c>
       <c r="I347" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B348" t="s">
         <v>316</v>
@@ -13260,12 +13322,12 @@
         <v>508</v>
       </c>
       <c r="I348" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B349" t="s">
         <v>316</v>
@@ -13286,12 +13348,12 @@
         <v>508</v>
       </c>
       <c r="I349" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B350" t="s">
         <v>316</v>
@@ -13312,12 +13374,12 @@
         <v>508</v>
       </c>
       <c r="I350" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B351" t="s">
         <v>316</v>
@@ -13338,12 +13400,12 @@
         <v>508</v>
       </c>
       <c r="I351" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B352" t="s">
         <v>316</v>
@@ -13364,7 +13426,7 @@
         <v>508</v>
       </c>
       <c r="I352" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.3">
@@ -13398,7 +13460,7 @@
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B354" t="s">
         <v>318</v>
@@ -13427,7 +13489,7 @@
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B355" t="s">
         <v>318</v>
@@ -13456,7 +13518,7 @@
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B356" t="s">
         <v>318</v>
@@ -13485,7 +13547,7 @@
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B357" t="s">
         <v>318</v>
@@ -13514,7 +13576,7 @@
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B358" t="s">
         <v>318</v>
@@ -13543,7 +13605,7 @@
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B359" t="s">
         <v>318</v>
@@ -13572,7 +13634,7 @@
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B360" t="s">
         <v>318</v>
@@ -13601,7 +13663,7 @@
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B361" t="s">
         <v>318</v>
@@ -13630,7 +13692,7 @@
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B362" t="s">
         <v>318</v>
@@ -13659,7 +13721,7 @@
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B363" t="s">
         <v>318</v>
@@ -13688,7 +13750,7 @@
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B364" t="s">
         <v>318</v>
@@ -13717,7 +13779,7 @@
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B365" t="s">
         <v>318</v>
@@ -13746,7 +13808,7 @@
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B366" t="s">
         <v>318</v>
@@ -13960,18 +14022,18 @@
         <v>341</v>
       </c>
       <c r="G374" s="2" t="s">
-        <v>508</v>
+        <v>939</v>
       </c>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
+        <v>862</v>
+      </c>
+      <c r="B375" t="s">
+        <v>862</v>
+      </c>
+      <c r="C375" t="s">
         <v>863</v>
-      </c>
-      <c r="B375" t="s">
-        <v>863</v>
-      </c>
-      <c r="C375" t="s">
-        <v>864</v>
       </c>
       <c r="D375" t="s">
         <v>3</v>
@@ -13986,10 +14048,10 @@
         <v>508</v>
       </c>
       <c r="H375" t="s">
+        <v>931</v>
+      </c>
+      <c r="I375" t="s">
         <v>932</v>
-      </c>
-      <c r="I375" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.3">
@@ -14023,13 +14085,13 @@
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
+        <v>864</v>
+      </c>
+      <c r="B377" t="s">
+        <v>864</v>
+      </c>
+      <c r="C377" t="s">
         <v>865</v>
-      </c>
-      <c r="B377" t="s">
-        <v>865</v>
-      </c>
-      <c r="C377" t="s">
-        <v>866</v>
       </c>
       <c r="D377" t="s">
         <v>3</v>
@@ -14047,18 +14109,18 @@
         <v>514</v>
       </c>
       <c r="I377" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
+        <v>866</v>
+      </c>
+      <c r="B378" t="s">
+        <v>866</v>
+      </c>
+      <c r="C378" t="s">
         <v>867</v>
-      </c>
-      <c r="B378" t="s">
-        <v>867</v>
-      </c>
-      <c r="C378" t="s">
-        <v>868</v>
       </c>
       <c r="D378" t="s">
         <v>3</v>
@@ -14073,21 +14135,21 @@
         <v>681</v>
       </c>
       <c r="H378" t="s">
+        <v>934</v>
+      </c>
+      <c r="I378" t="s">
         <v>935</v>
-      </c>
-      <c r="I378" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
+        <v>868</v>
+      </c>
+      <c r="B379" t="s">
+        <v>868</v>
+      </c>
+      <c r="C379" t="s">
         <v>869</v>
-      </c>
-      <c r="B379" t="s">
-        <v>869</v>
-      </c>
-      <c r="C379" t="s">
-        <v>870</v>
       </c>
       <c r="D379" t="s">
         <v>3</v>
@@ -14102,21 +14164,21 @@
         <v>508</v>
       </c>
       <c r="H379" t="s">
+        <v>936</v>
+      </c>
+      <c r="I379" t="s">
         <v>937</v>
-      </c>
-      <c r="I379" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="380" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
+        <v>870</v>
+      </c>
+      <c r="B380" t="s">
+        <v>870</v>
+      </c>
+      <c r="C380" t="s">
         <v>871</v>
-      </c>
-      <c r="B380" t="s">
-        <v>871</v>
-      </c>
-      <c r="C380" t="s">
-        <v>872</v>
       </c>
       <c r="D380" t="s">
         <v>3</v>
@@ -14128,10 +14190,10 @@
         <v>341</v>
       </c>
       <c r="G380" s="2" t="s">
-        <v>524</v>
+        <v>941</v>
       </c>
       <c r="I380" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.3">
@@ -14231,13 +14293,13 @@
     </row>
     <row r="385" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
+        <v>872</v>
+      </c>
+      <c r="B385" t="s">
         <v>873</v>
       </c>
-      <c r="B385" t="s">
+      <c r="C385" t="s">
         <v>874</v>
-      </c>
-      <c r="C385" t="s">
-        <v>875</v>
       </c>
       <c r="D385" t="s">
         <v>350</v>
@@ -14295,7 +14357,7 @@
         <v>10</v>
       </c>
       <c r="G387" t="s">
-        <v>940</v>
+        <v>15</v>
       </c>
     </row>
     <row r="388" spans="1:9" x14ac:dyDescent="0.3">
@@ -14438,13 +14500,13 @@
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
+        <v>875</v>
+      </c>
+      <c r="B394" t="s">
         <v>876</v>
       </c>
-      <c r="B394" t="s">
+      <c r="C394" t="s">
         <v>877</v>
-      </c>
-      <c r="C394" t="s">
-        <v>878</v>
       </c>
       <c r="D394" t="s">
         <v>350</v>
@@ -14461,13 +14523,13 @@
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
+        <v>878</v>
+      </c>
+      <c r="B395" t="s">
         <v>879</v>
       </c>
-      <c r="B395" t="s">
+      <c r="C395" t="s">
         <v>880</v>
-      </c>
-      <c r="C395" t="s">
-        <v>881</v>
       </c>
       <c r="D395" t="s">
         <v>350</v>
@@ -14648,13 +14710,13 @@
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
+        <v>881</v>
+      </c>
+      <c r="B403" t="s">
+        <v>881</v>
+      </c>
+      <c r="C403" t="s">
         <v>882</v>
-      </c>
-      <c r="B403" t="s">
-        <v>882</v>
-      </c>
-      <c r="C403" t="s">
-        <v>883</v>
       </c>
       <c r="D403" t="s">
         <v>15</v>
@@ -14775,13 +14837,13 @@
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
+        <v>883</v>
+      </c>
+      <c r="B408" t="s">
         <v>884</v>
       </c>
-      <c r="B408" t="s">
+      <c r="C408" t="s">
         <v>885</v>
-      </c>
-      <c r="C408" t="s">
-        <v>886</v>
       </c>
       <c r="D408" t="s">
         <v>15</v>
@@ -15419,13 +15481,13 @@
     </row>
     <row r="436" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
+        <v>886</v>
+      </c>
+      <c r="B436" t="s">
         <v>887</v>
       </c>
-      <c r="B436" t="s">
+      <c r="C436" t="s">
         <v>888</v>
-      </c>
-      <c r="C436" t="s">
-        <v>889</v>
       </c>
       <c r="D436" t="s">
         <v>15</v>
@@ -15465,13 +15527,13 @@
     </row>
     <row r="438" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
+        <v>889</v>
+      </c>
+      <c r="B438" t="s">
         <v>890</v>
       </c>
-      <c r="B438" t="s">
+      <c r="C438" t="s">
         <v>891</v>
-      </c>
-      <c r="C438" t="s">
-        <v>892</v>
       </c>
       <c r="D438" t="s">
         <v>15</v>
@@ -15488,13 +15550,13 @@
     </row>
     <row r="439" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
+        <v>892</v>
+      </c>
+      <c r="B439" t="s">
         <v>893</v>
       </c>
-      <c r="B439" t="s">
+      <c r="C439" t="s">
         <v>894</v>
-      </c>
-      <c r="C439" t="s">
-        <v>895</v>
       </c>
       <c r="D439" t="s">
         <v>15</v>
@@ -15580,13 +15642,13 @@
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
+        <v>895</v>
+      </c>
+      <c r="B443" t="s">
         <v>896</v>
       </c>
-      <c r="B443" t="s">
+      <c r="C443" t="s">
         <v>897</v>
-      </c>
-      <c r="C443" t="s">
-        <v>898</v>
       </c>
       <c r="D443" t="s">
         <v>15</v>
@@ -15606,10 +15668,10 @@
         <v>334</v>
       </c>
       <c r="B444" t="s">
+        <v>898</v>
+      </c>
+      <c r="C444" t="s">
         <v>899</v>
-      </c>
-      <c r="C444" t="s">
-        <v>900</v>
       </c>
       <c r="D444" t="s">
         <v>15</v>
@@ -15626,13 +15688,13 @@
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
+        <v>900</v>
+      </c>
+      <c r="B445" t="s">
         <v>901</v>
       </c>
-      <c r="B445" t="s">
-        <v>902</v>
-      </c>
       <c r="C445" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D445" t="s">
         <v>15</v>
@@ -15672,13 +15734,13 @@
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
+        <v>902</v>
+      </c>
+      <c r="B447" t="s">
         <v>903</v>
       </c>
-      <c r="B447" t="s">
+      <c r="C447" t="s">
         <v>904</v>
-      </c>
-      <c r="C447" t="s">
-        <v>905</v>
       </c>
       <c r="D447" t="s">
         <v>15</v>

</xml_diff>